<commit_message>
added synonyms to CRO and notes to spreadsheet.
</commit_message>
<xml_diff>
--- a/docs/CRO_draft_March26(1).xlsx
+++ b/docs/CRO_draft_March26(1).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haendel/Documents/GitHub/cd2h git/contributor-role-ontology/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vasilevs/git/contributor-role-ontology/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="27140" windowHeight="16540" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="27140" windowHeight="16240" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CRediT-original" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="139">
   <si>
     <t>Contributor Role</t>
   </si>
@@ -440,6 +443,9 @@
   </si>
   <si>
     <t>software enginnering</t>
+  </si>
+  <si>
+    <t>Notes - NV 10/01/18</t>
   </si>
 </sst>
 </file>
@@ -1178,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IZ108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,8 +1193,9 @@
     <col min="1" max="1" width="31.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="39.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:260" ht="19" x14ac:dyDescent="0.25">
@@ -1271,6 +1278,9 @@
       </c>
       <c r="E11" s="11" t="s">
         <v>36</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:260" s="10" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added new classes from CR-ProjectLevel tab
</commit_message>
<xml_diff>
--- a/docs/CRO_draft_March26(1).xlsx
+++ b/docs/CRO_draft_March26(1).xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="192">
   <si>
     <t>Contributor Role</t>
   </si>
@@ -477,6 +477,135 @@
   <si>
     <t>added as child of 'methodology role'</t>
   </si>
+  <si>
+    <t>CRO_0000035</t>
+  </si>
+  <si>
+    <t>added statistical analysis role as a syn</t>
+  </si>
+  <si>
+    <t>CRO_0000074</t>
+  </si>
+  <si>
+    <t>CRO_0000044</t>
+  </si>
+  <si>
+    <t>CRO_0000075</t>
+  </si>
+  <si>
+    <t>CRO_0000047</t>
+  </si>
+  <si>
+    <t>Relabled 'teaching role' and made 'teaching role' a syn</t>
+  </si>
+  <si>
+    <t>CRO_0000045</t>
+  </si>
+  <si>
+    <t>CRO_0000046</t>
+  </si>
+  <si>
+    <t>CRO_0000076</t>
+  </si>
+  <si>
+    <t>added a child of 'contributor role' - should these be two classes?</t>
+  </si>
+  <si>
+    <t>CRO_0000077</t>
+  </si>
+  <si>
+    <t>CRO_0000008</t>
+  </si>
+  <si>
+    <t>should this be a child of 'IT hardware systems design and implementation role'?</t>
+  </si>
+  <si>
+    <t>CRO_0000006</t>
+  </si>
+  <si>
+    <t>CRO_0000050</t>
+  </si>
+  <si>
+    <t>CRO_0000017</t>
+  </si>
+  <si>
+    <t>CRO_0000079</t>
+  </si>
+  <si>
+    <t>CRO_0000080</t>
+  </si>
+  <si>
+    <t>CRO_0000081</t>
+  </si>
+  <si>
+    <t>CRO_0000082</t>
+  </si>
+  <si>
+    <t>added as child of 'infrastructure role' (new class)</t>
+  </si>
+  <si>
+    <t>CRO_0000057</t>
+  </si>
+  <si>
+    <t>CRO_0000058</t>
+  </si>
+  <si>
+    <t>CRO_0000029</t>
+  </si>
+  <si>
+    <t>added as syn for ''study investigation role'</t>
+  </si>
+  <si>
+    <t>CRO_0000021</t>
+  </si>
+  <si>
+    <t>added as syn for 'methodology development role'</t>
+  </si>
+  <si>
+    <t>CRO_0000053</t>
+  </si>
+  <si>
+    <t>added as syn for 'protocol creation role'</t>
+  </si>
+  <si>
+    <t>CRO_0000056</t>
+  </si>
+  <si>
+    <t>CRO_0000083</t>
+  </si>
+  <si>
+    <t>CRO_0000084</t>
+  </si>
+  <si>
+    <t>added as syn for 'communication role'</t>
+  </si>
+  <si>
+    <t>CRO_0000007</t>
+  </si>
+  <si>
+    <t>CRO_0000085</t>
+  </si>
+  <si>
+    <t>CRO_0000086</t>
+  </si>
+  <si>
+    <t>CRO_0000087</t>
+  </si>
+  <si>
+    <t>added as child of 'study investigation role'</t>
+  </si>
+  <si>
+    <t>CRO_0000062</t>
+  </si>
+  <si>
+    <t>CRO_0000060</t>
+  </si>
+  <si>
+    <t>CRO_0000063</t>
+  </si>
+  <si>
+    <t>CRO_0000064</t>
+  </si>
 </sst>
 </file>
 
@@ -748,7 +877,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -770,8 +899,108 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -812,8 +1041,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -824,6 +1055,56 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -834,6 +1115,56 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1279,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IZ108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3604,7 +3935,12 @@
       <c r="E22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="23" spans="1:260" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
@@ -3622,7 +3958,9 @@
       <c r="E23" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -3892,7 +4230,9 @@
         <v>25</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="F24" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
@@ -4161,6 +4501,12 @@
       <c r="E25" s="7" t="s">
         <v>94</v>
       </c>
+      <c r="F25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="26" spans="1:260" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
@@ -4175,6 +4521,9 @@
       <c r="E26" s="7" t="s">
         <v>53</v>
       </c>
+      <c r="F26" s="7" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="27" spans="1:260" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
@@ -4189,6 +4538,9 @@
       <c r="E27" s="7" t="s">
         <v>53</v>
       </c>
+      <c r="F27" s="7" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="28" spans="1:260" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
@@ -4202,7 +4554,9 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>153</v>
+      </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -4472,8 +4826,12 @@
       <c r="E29" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F29"/>
-      <c r="G29" s="7"/>
+      <c r="F29" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>159</v>
+      </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -5012,7 +5370,9 @@
       <c r="E31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F31"/>
+      <c r="F31" t="s">
+        <v>160</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
@@ -5282,8 +5642,12 @@
       <c r="E32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F32"/>
-      <c r="G32" s="25"/>
+      <c r="F32" t="s">
+        <v>161</v>
+      </c>
+      <c r="G32" s="38" t="s">
+        <v>162</v>
+      </c>
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
@@ -5550,6 +5914,9 @@
       </c>
       <c r="E33" s="2" t="s">
         <v>53</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
@@ -5810,7 +6177,7 @@
       <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="40" t="s">
         <v>117</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -5820,8 +6187,12 @@
       <c r="E34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F34"/>
-      <c r="G34" s="7"/>
+      <c r="F34" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="38" t="s">
+        <v>139</v>
+      </c>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
@@ -6080,7 +6451,7 @@
       <c r="A35" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="41" t="s">
         <v>118</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -6092,7 +6463,9 @@
       <c r="E35" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="F35" s="8"/>
+      <c r="F35" s="8" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="36" spans="1:260" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
@@ -6646,8 +7019,12 @@
       </c>
       <c r="D38"/>
       <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38" s="7"/>
+      <c r="F38" t="s">
+        <v>166</v>
+      </c>
+      <c r="G38" s="38" t="s">
+        <v>170</v>
+      </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
@@ -6918,8 +7295,12 @@
       <c r="E39" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="10"/>
+      <c r="F39" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" s="38" t="s">
+        <v>170</v>
+      </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
@@ -7186,8 +7567,12 @@
       </c>
       <c r="D40"/>
       <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40" s="7"/>
+      <c r="F40" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" s="38" t="s">
+        <v>170</v>
+      </c>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
@@ -7726,8 +8111,12 @@
         <v>21</v>
       </c>
       <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="10"/>
+      <c r="F42" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="G42" s="38" t="s">
+        <v>170</v>
+      </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
@@ -7996,8 +8385,12 @@
       <c r="E43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="25"/>
+      <c r="F43" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>139</v>
+      </c>
       <c r="H43" s="25"/>
       <c r="I43" s="25"/>
       <c r="J43" s="25"/>
@@ -8266,7 +8659,9 @@
       <c r="E44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="G44" s="25"/>
       <c r="H44" s="25"/>
       <c r="I44" s="25"/>
@@ -8543,7 +8938,12 @@
       <c r="C46" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G46" s="25"/>
+      <c r="F46" t="s">
+        <v>173</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>174</v>
+      </c>
       <c r="H46" s="25"/>
       <c r="I46" s="25"/>
       <c r="J46" s="25"/>
@@ -9082,7 +9482,12 @@
         <v>13</v>
       </c>
       <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
+      <c r="F48" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="49" spans="1:260" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
@@ -9098,8 +9503,12 @@
       <c r="E49" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F49" s="2"/>
-      <c r="G49" s="25"/>
+      <c r="F49" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G49" s="38" t="s">
+        <v>178</v>
+      </c>
       <c r="H49" s="25"/>
       <c r="I49" s="25"/>
       <c r="J49" s="25"/>
@@ -9368,7 +9777,9 @@
       <c r="E50" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="G50" s="25"/>
       <c r="H50" s="25"/>
       <c r="I50" s="25"/>
@@ -9634,6 +10045,9 @@
       <c r="C51" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="F51" t="s">
+        <v>180</v>
+      </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
@@ -9901,7 +10315,9 @@
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
+      <c r="F52" s="7" t="s">
+        <v>181</v>
+      </c>
       <c r="G52" s="25"/>
       <c r="H52" s="25"/>
       <c r="I52" s="25"/>
@@ -10169,8 +10585,12 @@
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="25"/>
+      <c r="F53" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>182</v>
+      </c>
       <c r="H53" s="25"/>
       <c r="I53" s="25"/>
       <c r="J53" s="25"/>
@@ -10437,7 +10857,9 @@
       </c>
       <c r="D54"/>
       <c r="E54"/>
-      <c r="F54"/>
+      <c r="F54" t="s">
+        <v>184</v>
+      </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
@@ -10707,7 +11129,9 @@
         <v>3</v>
       </c>
       <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
+      <c r="F55" s="8" t="s">
+        <v>185</v>
+      </c>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
@@ -10973,6 +11397,9 @@
       <c r="C56" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="F56" t="s">
+        <v>168</v>
+      </c>
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
       <c r="I56" s="25"/>
@@ -11238,7 +11665,12 @@
       <c r="C57" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G57" s="25"/>
+      <c r="F57" t="s">
+        <v>186</v>
+      </c>
+      <c r="G57" s="25" t="s">
+        <v>187</v>
+      </c>
       <c r="H57" s="25"/>
       <c r="I57" s="25"/>
       <c r="J57" s="25"/>
@@ -11507,7 +11939,9 @@
       <c r="E58" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="G58" s="25"/>
       <c r="H58" s="25"/>
       <c r="I58" s="25"/>
@@ -11767,7 +12201,7 @@
       <c r="A59" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -11777,7 +12211,9 @@
       <c r="E59" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="G59" s="25"/>
       <c r="H59" s="25"/>
       <c r="I59" s="25"/>
@@ -12047,7 +12483,9 @@
       <c r="E60" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F60" s="2"/>
+      <c r="F60" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="G60" s="25"/>
       <c r="H60" s="25"/>
       <c r="I60" s="25"/>
@@ -12317,7 +12755,9 @@
       <c r="E61" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F61" s="2"/>
+      <c r="F61" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="G61" s="25"/>
       <c r="H61" s="25"/>
       <c r="I61" s="25"/>

</xml_diff>

<commit_message>
added new classes from CR-OutputLevel tab and added notes to spreadsheet
</commit_message>
<xml_diff>
--- a/docs/CRO_draft_March26(1).xlsx
+++ b/docs/CRO_draft_March26(1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="27140" windowHeight="16240" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="27140" windowHeight="16240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CRediT-original" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="207">
   <si>
     <t>Contributor Role</t>
   </si>
@@ -472,9 +472,6 @@
     <t>CRO_0000073</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>added as child of 'methodology role'</t>
   </si>
   <si>
@@ -605,6 +602,54 @@
   </si>
   <si>
     <t>CRO_0000064</t>
+  </si>
+  <si>
+    <t>NV notes 10/01/18</t>
+  </si>
+  <si>
+    <t>CRO_0000088</t>
+  </si>
+  <si>
+    <t>CRO_0000089</t>
+  </si>
+  <si>
+    <t>CRO_0000002</t>
+  </si>
+  <si>
+    <t>added as syn</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>CRO_0000014</t>
+  </si>
+  <si>
+    <t>CRO_0000090</t>
+  </si>
+  <si>
+    <t>CRO_0000020</t>
+  </si>
+  <si>
+    <t>moved to child of 'infrastructure role'</t>
+  </si>
+  <si>
+    <t>CRO_0000024</t>
+  </si>
+  <si>
+    <t>CRO_0000027</t>
+  </si>
+  <si>
+    <t>CRO_0000030</t>
+  </si>
+  <si>
+    <t>CRO_0000060, CRO_0000019</t>
+  </si>
+  <si>
+    <t>CRO_0000061</t>
+  </si>
+  <si>
+    <t>CRO_0000028</t>
   </si>
 </sst>
 </file>
@@ -877,7 +922,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -999,8 +1044,88 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1043,8 +1168,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="201">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1105,6 +1231,46 @@
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1165,6 +1331,46 @@
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1610,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:IZ108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1706,10 +1912,10 @@
         <v>36</v>
       </c>
       <c r="F11" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:260" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -1724,7 +1930,9 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
@@ -1995,7 +2203,7 @@
         <v>83</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -3354,8 +3562,12 @@
         <v>7</v>
       </c>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>195</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -3918,7 +4130,7 @@
         <v>146</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:260" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3936,10 +4148,10 @@
         <v>46</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G22" s="38" t="s">
         <v>149</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:260" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -3959,7 +4171,7 @@
         <v>47</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -4231,7 +4443,7 @@
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -4502,10 +4714,10 @@
         <v>94</v>
       </c>
       <c r="F25" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" s="38" t="s">
         <v>154</v>
-      </c>
-      <c r="G25" s="38" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:260" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4522,7 +4734,7 @@
         <v>53</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:260" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4539,7 +4751,7 @@
         <v>53</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:260" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -4555,7 +4767,7 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -4827,10 +5039,10 @@
         <v>53</v>
       </c>
       <c r="F29" t="s">
+        <v>157</v>
+      </c>
+      <c r="G29" s="38" t="s">
         <v>158</v>
-      </c>
-      <c r="G29" s="38" t="s">
-        <v>159</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -5371,7 +5583,7 @@
         <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
@@ -5643,10 +5855,10 @@
         <v>56</v>
       </c>
       <c r="F32" t="s">
+        <v>160</v>
+      </c>
+      <c r="G32" s="38" t="s">
         <v>161</v>
-      </c>
-      <c r="G32" s="38" t="s">
-        <v>162</v>
       </c>
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
@@ -5916,7 +6128,7 @@
         <v>53</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
@@ -6188,7 +6400,7 @@
         <v>56</v>
       </c>
       <c r="F34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G34" s="38" t="s">
         <v>139</v>
@@ -6464,7 +6676,7 @@
         <v>90</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:260" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -7020,10 +7232,10 @@
       <c r="D38"/>
       <c r="E38"/>
       <c r="F38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G38" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
@@ -7296,10 +7508,10 @@
         <v>90</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G39" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -7568,10 +7780,10 @@
       <c r="D40"/>
       <c r="E40"/>
       <c r="F40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G40" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
@@ -8112,10 +8324,10 @@
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G42" s="38" t="s">
         <v>169</v>
-      </c>
-      <c r="G42" s="38" t="s">
-        <v>170</v>
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
@@ -8386,7 +8598,7 @@
         <v>43</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G43" s="38" t="s">
         <v>139</v>
@@ -8660,7 +8872,7 @@
         <v>43</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G44" s="25"/>
       <c r="H44" s="25"/>
@@ -8939,10 +9151,10 @@
         <v>86</v>
       </c>
       <c r="F46" t="s">
+        <v>172</v>
+      </c>
+      <c r="G46" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="G46" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="H46" s="25"/>
       <c r="I46" s="25"/>
@@ -9483,10 +9695,10 @@
       </c>
       <c r="E48" s="10"/>
       <c r="F48" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="G48" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:260" x14ac:dyDescent="0.2">
@@ -9504,10 +9716,10 @@
         <v>43</v>
       </c>
       <c r="F49" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G49" s="38" t="s">
         <v>177</v>
-      </c>
-      <c r="G49" s="38" t="s">
-        <v>178</v>
       </c>
       <c r="H49" s="25"/>
       <c r="I49" s="25"/>
@@ -9778,7 +9990,7 @@
         <v>43</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G50" s="25"/>
       <c r="H50" s="25"/>
@@ -10046,7 +10258,7 @@
         <v>70</v>
       </c>
       <c r="F51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -10316,7 +10528,7 @@
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G52" s="25"/>
       <c r="H52" s="25"/>
@@ -10586,10 +10798,10 @@
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G53" s="25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H53" s="25"/>
       <c r="I53" s="25"/>
@@ -10858,7 +11070,7 @@
       <c r="D54"/>
       <c r="E54"/>
       <c r="F54" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -11130,7 +11342,7 @@
       </c>
       <c r="E55" s="8"/>
       <c r="F55" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
@@ -11398,7 +11610,7 @@
         <v>88</v>
       </c>
       <c r="F56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
@@ -11666,10 +11878,10 @@
         <v>60</v>
       </c>
       <c r="F57" t="s">
+        <v>185</v>
+      </c>
+      <c r="G57" s="25" t="s">
         <v>186</v>
-      </c>
-      <c r="G57" s="25" t="s">
-        <v>187</v>
       </c>
       <c r="H57" s="25"/>
       <c r="I57" s="25"/>
@@ -11940,7 +12152,7 @@
         <v>43</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G58" s="25"/>
       <c r="H58" s="25"/>
@@ -12212,7 +12424,7 @@
         <v>43</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G59" s="25"/>
       <c r="H59" s="25"/>
@@ -12484,7 +12696,7 @@
         <v>43</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G60" s="25"/>
       <c r="H60" s="25"/>
@@ -12756,7 +12968,7 @@
         <v>43</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G61" s="25"/>
       <c r="H61" s="25"/>
@@ -24827,8 +25039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IY66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24837,7 +25049,8 @@
     <col min="2" max="2" width="39.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="34.5" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:259" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -24883,6 +25096,12 @@
       <c r="D9" s="11" t="s">
         <v>36</v>
       </c>
+      <c r="E9" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="10" spans="1:259" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
@@ -24893,7 +25112,9 @@
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>193</v>
+      </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
@@ -25159,6 +25380,9 @@
       <c r="C11" s="26" t="s">
         <v>27</v>
       </c>
+      <c r="E11" s="26" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="12" spans="1:259" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
@@ -25170,6 +25394,12 @@
       <c r="C12" s="26" t="s">
         <v>29</v>
       </c>
+      <c r="E12" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="13" spans="1:259" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
@@ -25182,8 +25412,12 @@
       <c r="D13" t="s">
         <v>83</v>
       </c>
-      <c r="E13"/>
-      <c r="F13" s="7"/>
+      <c r="E13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>195</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -25449,7 +25683,9 @@
       <c r="D14" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -25716,8 +25952,12 @@
         <v>5</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>195</v>
+      </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -25983,7 +26223,9 @@
       <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -26250,7 +26492,9 @@
       <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
@@ -26517,7 +26761,9 @@
         <v>7</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>140</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -26784,7 +27030,9 @@
         <v>73</v>
       </c>
       <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -27051,7 +27299,9 @@
       <c r="D20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>145</v>
+      </c>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
@@ -27320,7 +27570,9 @@
       <c r="D21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -27587,7 +27839,9 @@
       <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
@@ -27856,7 +28110,9 @@
       <c r="D23" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -28123,7 +28379,9 @@
         <v>25</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -28390,8 +28648,12 @@
       <c r="D25" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>195</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -28657,7 +28919,9 @@
       <c r="D26" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>155</v>
+      </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
@@ -28924,7 +29188,9 @@
       <c r="D27" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="7" t="s">
+        <v>156</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -29189,8 +29455,12 @@
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
+      <c r="E28" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="38" t="s">
+        <v>195</v>
+      </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -29456,7 +29726,9 @@
       <c r="D29" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E29"/>
+      <c r="E29" t="s">
+        <v>157</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -29723,7 +29995,9 @@
       <c r="D30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E30"/>
+      <c r="E30" t="s">
+        <v>157</v>
+      </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -29990,7 +30264,9 @@
       <c r="D31" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E31"/>
+      <c r="E31" t="s">
+        <v>159</v>
+      </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
@@ -30257,7 +30533,9 @@
       <c r="D32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E32"/>
+      <c r="E32" t="s">
+        <v>198</v>
+      </c>
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
@@ -30524,7 +30802,9 @@
       <c r="D33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
@@ -30791,7 +31071,9 @@
       <c r="D34" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E34"/>
+      <c r="E34" t="s">
+        <v>163</v>
+      </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -31060,6 +31342,9 @@
       <c r="D35" s="22" t="s">
         <v>90</v>
       </c>
+      <c r="E35" s="8" t="s">
+        <v>164</v>
+      </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -31326,7 +31611,9 @@
       <c r="D36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E36"/>
+      <c r="E36" t="s">
+        <v>199</v>
+      </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
@@ -31593,8 +31880,12 @@
       <c r="D37" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E37"/>
-      <c r="F37" s="7"/>
+      <c r="E37" t="s">
+        <v>199</v>
+      </c>
+      <c r="F37" s="38" t="s">
+        <v>200</v>
+      </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
@@ -31858,7 +32149,9 @@
       </c>
       <c r="C38"/>
       <c r="D38"/>
-      <c r="E38"/>
+      <c r="E38" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="39" spans="1:259" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
@@ -31873,7 +32166,9 @@
       <c r="D39" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="8"/>
+      <c r="E39" s="8" t="s">
+        <v>201</v>
+      </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
@@ -32138,7 +32433,9 @@
       </c>
       <c r="C40"/>
       <c r="D40"/>
-      <c r="E40"/>
+      <c r="E40" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="41" spans="1:259" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
@@ -32151,7 +32448,9 @@
         <v>17</v>
       </c>
       <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="E41" s="8" t="s">
+        <v>202</v>
+      </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
@@ -32418,7 +32717,9 @@
         <v>21</v>
       </c>
       <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8" t="s">
+        <v>203</v>
+      </c>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -32685,7 +32986,9 @@
       <c r="D43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E43" s="2"/>
+      <c r="E43" s="40" t="s">
+        <v>170</v>
+      </c>
       <c r="F43" s="25"/>
       <c r="G43" s="25"/>
       <c r="H43" s="25"/>
@@ -32951,6 +33254,9 @@
       <c r="D44" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E44" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
       <c r="H44" s="25"/>
@@ -33215,7 +33521,9 @@
       </c>
       <c r="C45" s="20"/>
       <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
+      <c r="E45" s="20" t="s">
+        <v>142</v>
+      </c>
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
       <c r="H45" s="25"/>
@@ -33480,7 +33788,9 @@
       </c>
       <c r="C46"/>
       <c r="D46"/>
-      <c r="E46"/>
+      <c r="E46" t="s">
+        <v>172</v>
+      </c>
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
       <c r="H46" s="25"/>
@@ -33747,7 +34057,9 @@
         <v>11</v>
       </c>
       <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="E47" t="s">
+        <v>172</v>
+      </c>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
@@ -34013,6 +34325,9 @@
       <c r="C48" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="E48" s="10" t="s">
+        <v>174</v>
+      </c>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
@@ -34279,7 +34594,9 @@
       <c r="D49" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
       <c r="H49" s="25"/>
@@ -34545,6 +34862,9 @@
       <c r="D50" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="E50" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
       <c r="H50" s="25"/>
@@ -34809,7 +35129,9 @@
       </c>
       <c r="C51"/>
       <c r="D51"/>
-      <c r="E51"/>
+      <c r="E51" t="s">
+        <v>179</v>
+      </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
@@ -35074,7 +35396,9 @@
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
+      <c r="E52" s="7" t="s">
+        <v>180</v>
+      </c>
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
       <c r="H52" s="25"/>
@@ -35339,7 +35663,9 @@
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
+      <c r="E53" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="25"/>
@@ -35604,7 +35930,9 @@
       </c>
       <c r="C54"/>
       <c r="D54"/>
-      <c r="E54"/>
+      <c r="E54" t="s">
+        <v>183</v>
+      </c>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
@@ -35871,7 +36199,9 @@
         <v>3</v>
       </c>
       <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="E55" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="F55" s="8"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
@@ -36136,7 +36466,9 @@
       </c>
       <c r="C56"/>
       <c r="D56"/>
-      <c r="E56"/>
+      <c r="E56" t="s">
+        <v>167</v>
+      </c>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
@@ -36399,6 +36731,9 @@
       <c r="B57" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="E57" t="s">
+        <v>185</v>
+      </c>
       <c r="F57" s="25"/>
       <c r="G57" s="25"/>
       <c r="H57" s="25"/>
@@ -36665,7 +37000,9 @@
       <c r="D58" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="F58" s="25"/>
       <c r="G58" s="25"/>
       <c r="H58" s="25"/>
@@ -36932,7 +37269,9 @@
       <c r="D59" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E59" s="2"/>
+      <c r="E59" s="40" t="s">
+        <v>204</v>
+      </c>
       <c r="F59" s="25"/>
       <c r="G59" s="25"/>
       <c r="H59" s="25"/>
@@ -37199,7 +37538,9 @@
       <c r="D60" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E60" s="2"/>
+      <c r="E60" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="F60" s="25"/>
       <c r="G60" s="25"/>
       <c r="H60" s="25"/>
@@ -37466,7 +37807,9 @@
       <c r="D61" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="F61" s="25"/>
       <c r="G61" s="25"/>
       <c r="H61" s="25"/>
@@ -37733,7 +38076,9 @@
       <c r="D62" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="F62" s="25"/>
       <c r="G62" s="25"/>
       <c r="H62" s="25"/>
@@ -37998,6 +38343,9 @@
       </c>
       <c r="C63" s="10" t="s">
         <v>19</v>
+      </c>
+      <c r="E63" s="8" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:259" s="8" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>